<commit_message>
Update XLSX stub file used for unit tests (due to refactoring id->name)
</commit_message>
<xml_diff>
--- a/reqcoco-parser-xlsx/src/test/resources/samples/input/req_declarations_1.xlsx
+++ b/reqcoco-parser-xlsx/src/test/resources/samples/input/req_declarations_1.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Donnees\B0021603\Dev\workspaces\workspaces_drafts\reqcoco-parent\reqcoco-generator-xlsx\src\test\resources\samples\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paissad/Documents/workspaces/workspace_drafts/reqcoco-parent/reqcoco-parser-xlsx/src/test/resources/samples/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="8085"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17900" windowHeight="8080"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,9 +32,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>version</t>
   </si>
   <si>
@@ -48,12 +51,15 @@
   </si>
   <si>
     <t xml:space="preserve">req_14 desc !  </t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -370,43 +376,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="1" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" style="1"/>
-    <col min="4" max="4" width="50.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="50.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>